<commit_message>
added time bounds with time of day type
</commit_message>
<xml_diff>
--- a/Data/Article/Endpoints.xlsx
+++ b/Data/Article/Endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ilya\Documents\Projects\HAQuDA\Data\Article\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4745F9D-EDA6-4F94-A32A-BD05C46F1B08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BE5D3D-2B52-4F68-B191-F0A8EE975E61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-5310" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="73">
   <si>
     <t>Basic cluster
 0x0000 (0)</t>
@@ -228,15 +228,9 @@
     <t>Time bounds  0xfc04 (64516) (CUSTOM)</t>
   </si>
   <si>
-    <t>UpperBound</t>
-  </si>
-  <si>
     <t>TimeZone</t>
   </si>
   <si>
-    <t>LowerBound</t>
-  </si>
-  <si>
     <t>0x001D</t>
   </si>
   <si>
@@ -244,6 +238,18 @@
   </si>
   <si>
     <t>0x00000000</t>
+  </si>
+  <si>
+    <t>UpperBound (in minutes from midnight)</t>
+  </si>
+  <si>
+    <t>LowerBound (in minutes from midnight)</t>
+  </si>
+  <si>
+    <t>0x021C (09:00 AM)</t>
+  </si>
+  <si>
+    <t>0x04EC (09:00 PM)</t>
   </si>
 </sst>
 </file>
@@ -312,7 +318,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,6 +335,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -492,7 +504,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -562,69 +574,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -911,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y30" sqref="Y30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -931,7 +940,7 @@
     <col min="16" max="16" width="19.6640625" customWidth="1"/>
     <col min="19" max="19" width="16" customWidth="1"/>
     <col min="20" max="20" width="12.21875" customWidth="1"/>
-    <col min="21" max="21" width="18.88671875" customWidth="1"/>
+    <col min="21" max="21" width="21.5546875" customWidth="1"/>
     <col min="22" max="22" width="19.6640625" customWidth="1"/>
     <col min="25" max="26" width="16" customWidth="1"/>
     <col min="27" max="27" width="21.109375" customWidth="1"/>
@@ -939,30 +948,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="G1" s="26" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="G1" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="M1" s="26" t="s">
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="M1" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="S1" s="26" t="s">
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="S1" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="42"/>
+      <c r="V1" s="42"/>
       <c r="Y1" s="18" t="s">
         <v>46</v>
       </c>
@@ -974,11 +983,11 @@
       <c r="A2" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
       <c r="G2" s="12" t="s">
         <v>56</v>
       </c>
@@ -1037,7 +1046,7 @@
       <c r="J3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="25" t="s">
+      <c r="M3" s="36" t="s">
         <v>0</v>
       </c>
       <c r="N3" s="3" t="s">
@@ -1095,7 +1104,7 @@
       <c r="J4" s="4">
         <v>2</v>
       </c>
-      <c r="M4" s="25"/>
+      <c r="M4" s="36"/>
       <c r="N4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1147,7 +1156,7 @@
       <c r="J5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="25"/>
+      <c r="M5" s="36"/>
       <c r="N5" s="4" t="s">
         <v>5</v>
       </c>
@@ -1199,7 +1208,7 @@
       <c r="J6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="25"/>
+      <c r="M6" s="36"/>
       <c r="N6" s="4" t="s">
         <v>6</v>
       </c>
@@ -1251,7 +1260,7 @@
       <c r="J7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="25"/>
+      <c r="M7" s="36"/>
       <c r="N7" s="4" t="s">
         <v>7</v>
       </c>
@@ -1303,7 +1312,7 @@
       <c r="J8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="25"/>
+      <c r="M8" s="36"/>
       <c r="N8" s="4" t="s">
         <v>8</v>
       </c>
@@ -1355,7 +1364,7 @@
       <c r="J9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M9" s="25"/>
+      <c r="M9" s="36"/>
       <c r="N9" s="4" t="s">
         <v>9</v>
       </c>
@@ -1501,7 +1510,7 @@
       </c>
     </row>
     <row r="12" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="36" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1563,7 +1572,7 @@
       </c>
     </row>
     <row r="13" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="4" t="s">
         <v>4</v>
       </c>
@@ -1615,7 +1624,7 @@
       </c>
     </row>
     <row r="14" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="40" t="s">
         <v>58</v>
       </c>
       <c r="B14" s="11" t="s">
@@ -1671,14 +1680,14 @@
       </c>
     </row>
     <row r="15" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27"/>
-      <c r="B15" s="33" t="s">
+      <c r="A15" s="40"/>
+      <c r="B15" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="36" t="s">
         <v>62</v>
       </c>
       <c r="G15" s="23"/>
@@ -1723,10 +1732,10 @@
       </c>
     </row>
     <row r="16" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="25"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="36"/>
       <c r="G16" s="24"/>
       <c r="H16" s="4" t="s">
         <v>33</v>
@@ -1769,10 +1778,10 @@
       </c>
     </row>
     <row r="17" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="27"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="25"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="36"/>
       <c r="G17" s="22" t="s">
         <v>59</v>
       </c>
@@ -1785,7 +1794,7 @@
       <c r="J17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M17" s="36" t="s">
+      <c r="M17" s="33" t="s">
         <v>60</v>
       </c>
       <c r="N17" s="11" t="s">
@@ -1822,23 +1831,23 @@
     </row>
     <row r="18" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G18" s="23"/>
-      <c r="H18" s="33" t="s">
+      <c r="H18" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="I18" s="33" t="s">
+      <c r="I18" s="31" t="s">
         <v>39</v>
       </c>
       <c r="J18" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="M18" s="37"/>
-      <c r="N18" s="33" t="s">
+      <c r="M18" s="34"/>
+      <c r="N18" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="O18" s="33" t="s">
+      <c r="O18" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="P18" s="25" t="s">
+      <c r="P18" s="36" t="s">
         <v>40</v>
       </c>
       <c r="S18" s="24"/>
@@ -1864,13 +1873,13 @@
     </row>
     <row r="19" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G19" s="23"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
       <c r="J19" s="23"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="33"/>
-      <c r="O19" s="33"/>
-      <c r="P19" s="25"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="36"/>
       <c r="S19" s="22" t="s">
         <v>59</v>
       </c>
@@ -1896,18 +1905,18 @@
     </row>
     <row r="20" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G20" s="23"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
       <c r="J20" s="23"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
-      <c r="P20" s="25"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="36"/>
       <c r="S20" s="23"/>
-      <c r="T20" s="29" t="s">
+      <c r="T20" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="U20" s="31" t="s">
+      <c r="U20" s="28" t="s">
         <v>39</v>
       </c>
       <c r="V20" s="22" t="s">
@@ -1926,16 +1935,16 @@
     </row>
     <row r="21" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G21" s="24"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
       <c r="J21" s="24"/>
-      <c r="M21" s="38"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
-      <c r="P21" s="25"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="36"/>
       <c r="S21" s="23"/>
-      <c r="T21" s="30"/>
-      <c r="U21" s="32"/>
+      <c r="T21" s="26"/>
+      <c r="U21" s="29"/>
       <c r="V21" s="23"/>
       <c r="Y21" s="23"/>
       <c r="Z21" s="2" t="s">
@@ -1949,7 +1958,7 @@
       </c>
     </row>
     <row r="22" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="M22" s="25" t="s">
+      <c r="M22" s="36" t="s">
         <v>63</v>
       </c>
       <c r="N22" s="11" t="s">
@@ -1962,8 +1971,8 @@
         <v>3</v>
       </c>
       <c r="S22" s="23"/>
-      <c r="T22" s="30"/>
-      <c r="U22" s="32"/>
+      <c r="T22" s="26"/>
+      <c r="U22" s="29"/>
       <c r="V22" s="23"/>
       <c r="Y22" s="24"/>
       <c r="Z22" s="2" t="s">
@@ -1977,46 +1986,46 @@
       </c>
     </row>
     <row r="23" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="M23" s="25"/>
-      <c r="N23" s="33" t="s">
+      <c r="M23" s="36"/>
+      <c r="N23" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="O23" s="34" t="s">
+      <c r="O23" s="37" t="s">
         <v>39</v>
       </c>
       <c r="P23" s="22" t="s">
         <v>42</v>
       </c>
       <c r="S23" s="23"/>
-      <c r="T23" s="30"/>
-      <c r="U23" s="32"/>
+      <c r="T23" s="26"/>
+      <c r="U23" s="29"/>
       <c r="V23" s="23"/>
     </row>
     <row r="24" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="M24" s="25"/>
-      <c r="N24" s="33"/>
-      <c r="O24" s="35"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="38"/>
       <c r="P24" s="23"/>
       <c r="S24" s="24"/>
-      <c r="T24" s="39"/>
-      <c r="U24" s="41"/>
+      <c r="T24" s="27"/>
+      <c r="U24" s="30"/>
       <c r="V24" s="24"/>
     </row>
     <row r="25" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="M25" s="25"/>
-      <c r="N25" s="33"/>
-      <c r="O25" s="35"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="31"/>
+      <c r="O25" s="38"/>
       <c r="P25" s="23"/>
-      <c r="S25" s="46" t="s">
+      <c r="S25" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="T25" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="U25" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="V25" s="44" t="s">
+      <c r="T25" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="U25" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="V25" s="45" t="s">
         <v>3</v>
       </c>
       <c r="Y25" s="1"/>
@@ -2025,18 +2034,20 @@
       <c r="AB25" s="1"/>
     </row>
     <row r="26" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="M26" s="25"/>
-      <c r="N26" s="33"/>
-      <c r="O26" s="40"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="31"/>
+      <c r="O26" s="39"/>
       <c r="P26" s="24"/>
-      <c r="S26" s="46"/>
-      <c r="T26" s="45" t="s">
+      <c r="S26" s="32"/>
+      <c r="T26" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="U26" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="V26" s="45"/>
+      <c r="U26" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="V26" s="43" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="27" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I27" s="1"/>
@@ -2055,14 +2066,10 @@
       <c r="P27" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="S27" s="46"/>
-      <c r="T27" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="U27" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="V27" s="45"/>
+      <c r="S27" s="32"/>
+      <c r="T27" s="43"/>
+      <c r="U27" s="32"/>
+      <c r="V27" s="43"/>
     </row>
     <row r="28" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I28" s="1"/>
@@ -2070,24 +2077,24 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="23"/>
-      <c r="N28" s="33" t="s">
+      <c r="N28" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="O28" s="33" t="s">
+      <c r="O28" s="31" t="s">
         <v>39</v>
       </c>
       <c r="P28" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="S28" s="46"/>
-      <c r="T28" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="U28" s="45" t="s">
+      <c r="S28" s="32"/>
+      <c r="T28" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="V28" s="45" t="s">
+      <c r="U28" s="32" t="s">
         <v>70</v>
+      </c>
+      <c r="V28" s="43" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2096,9 +2103,13 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="23"/>
-      <c r="N29" s="33"/>
-      <c r="O29" s="33"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="31"/>
       <c r="P29" s="23"/>
+      <c r="S29" s="32"/>
+      <c r="T29" s="43"/>
+      <c r="U29" s="32"/>
+      <c r="V29" s="43"/>
     </row>
     <row r="30" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I30" s="1"/>
@@ -2106,9 +2117,19 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="23"/>
-      <c r="N30" s="33"/>
-      <c r="O30" s="33"/>
+      <c r="N30" s="31"/>
+      <c r="O30" s="31"/>
       <c r="P30" s="23"/>
+      <c r="S30" s="32"/>
+      <c r="T30" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="U30" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="V30" s="44" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="31" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I31" s="1"/>
@@ -2116,8 +2137,8 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="24"/>
-      <c r="N31" s="33"/>
-      <c r="O31" s="33"/>
+      <c r="N31" s="31"/>
+      <c r="O31" s="31"/>
       <c r="P31" s="24"/>
     </row>
     <row r="32" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2259,30 +2280,23 @@
       <c r="D54" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="47">
-    <mergeCell ref="V20:V24"/>
-    <mergeCell ref="T20:T24"/>
-    <mergeCell ref="U20:U24"/>
-    <mergeCell ref="Y3:Y9"/>
-    <mergeCell ref="Y10:Y11"/>
-    <mergeCell ref="Y12:Y16"/>
-    <mergeCell ref="Y17:Y22"/>
-    <mergeCell ref="M27:M31"/>
-    <mergeCell ref="N28:N31"/>
-    <mergeCell ref="O28:O31"/>
-    <mergeCell ref="P28:P31"/>
-    <mergeCell ref="S3:S9"/>
-    <mergeCell ref="S10:S11"/>
-    <mergeCell ref="S12:S13"/>
-    <mergeCell ref="S14:S18"/>
-    <mergeCell ref="S19:S24"/>
-    <mergeCell ref="S25:S28"/>
-    <mergeCell ref="M17:M21"/>
-    <mergeCell ref="N18:N21"/>
-    <mergeCell ref="O18:O21"/>
-    <mergeCell ref="P18:P21"/>
-    <mergeCell ref="M22:M26"/>
-    <mergeCell ref="N23:N26"/>
+  <mergeCells count="53">
+    <mergeCell ref="S25:S30"/>
+    <mergeCell ref="U26:U27"/>
+    <mergeCell ref="T26:T27"/>
+    <mergeCell ref="V26:V27"/>
+    <mergeCell ref="U28:U29"/>
+    <mergeCell ref="T28:T29"/>
+    <mergeCell ref="V28:V29"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="M3:M9"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="M12:M16"/>
     <mergeCell ref="O23:O26"/>
     <mergeCell ref="P23:P26"/>
     <mergeCell ref="A14:A17"/>
@@ -2298,15 +2312,28 @@
     <mergeCell ref="H18:H21"/>
     <mergeCell ref="I18:I21"/>
     <mergeCell ref="B15:B17"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="M3:M9"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="M12:M16"/>
+    <mergeCell ref="M27:M31"/>
+    <mergeCell ref="N28:N31"/>
+    <mergeCell ref="O28:O31"/>
+    <mergeCell ref="P28:P31"/>
+    <mergeCell ref="S3:S9"/>
+    <mergeCell ref="S10:S11"/>
+    <mergeCell ref="S12:S13"/>
+    <mergeCell ref="S14:S18"/>
+    <mergeCell ref="S19:S24"/>
+    <mergeCell ref="M17:M21"/>
+    <mergeCell ref="N18:N21"/>
+    <mergeCell ref="O18:O21"/>
+    <mergeCell ref="P18:P21"/>
+    <mergeCell ref="M22:M26"/>
+    <mergeCell ref="N23:N26"/>
+    <mergeCell ref="V20:V24"/>
+    <mergeCell ref="T20:T24"/>
+    <mergeCell ref="U20:U24"/>
+    <mergeCell ref="Y3:Y9"/>
+    <mergeCell ref="Y10:Y11"/>
+    <mergeCell ref="Y12:Y16"/>
+    <mergeCell ref="Y17:Y22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>